<commit_message>
Module 5: create student.csv for testing and add display record functionality
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8090a3a5aa513dda/Desktop/DATA 200/Assignments/Data200-Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="8_{FAE45539-54BC-4D8E-88C3-6FEAF606C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5977E0AA-040A-4148-8C2B-0ADFA1F601F7}"/>
+  <xr:revisionPtr revIDLastSave="12" documentId="8_{FAE45539-54BC-4D8E-88C3-6FEAF606C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B9304B-F23A-4A38-BC96-DF7747C24B71}"/>
   <bookViews>
-    <workbookView xWindow="42465" yWindow="2820" windowWidth="19200" windowHeight="11715" xr2:uid="{001A2BA6-0299-40B0-A0C7-457F992103DF}"/>
+    <workbookView xWindow="42150" yWindow="3930" windowWidth="19200" windowHeight="10275" xr2:uid="{001A2BA6-0299-40B0-A0C7-457F992103DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>first_name</t>
   </si>
@@ -58,6 +58,18 @@
   </si>
   <si>
     <t>mae@myschool.edu</t>
+  </si>
+  <si>
+    <t>Sally</t>
+  </si>
+  <si>
+    <t>Russell</t>
+  </si>
+  <si>
+    <t>russell@myschool.edu</t>
+  </si>
+  <si>
+    <t>A-</t>
   </si>
 </sst>
 </file>
@@ -123,10 +135,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -164,7 +180,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -270,7 +286,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,7 +428,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -420,10 +436,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C6B5B9-B226-488D-8B04-AC508BAF3B03}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -476,9 +492,30 @@
         <v>88</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{61BB2DB2-4377-4FB7-A21D-AD9EE142CC00}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{08435CFB-1935-4089-AE0D-059F73C392E0}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Module 6: implement sorting of students, add more student data
</commit_message>
<xml_diff>
--- a/student.xlsx
+++ b/student.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8090a3a5aa513dda/Desktop/DATA 200/Assignments/Data200-Lab1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{FAE45539-54BC-4D8E-88C3-6FEAF606C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B9304B-F23A-4A38-BC96-DF7747C24B71}"/>
+  <xr:revisionPtr revIDLastSave="21" documentId="8_{FAE45539-54BC-4D8E-88C3-6FEAF606C31A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{99AA9816-F643-4712-8534-C94143A7CF6B}"/>
   <bookViews>
-    <workbookView xWindow="42150" yWindow="3930" windowWidth="19200" windowHeight="10275" xr2:uid="{001A2BA6-0299-40B0-A0C7-457F992103DF}"/>
+    <workbookView xWindow="38685" yWindow="2280" windowWidth="21600" windowHeight="11175" xr2:uid="{001A2BA6-0299-40B0-A0C7-457F992103DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="54">
   <si>
     <t>first_name</t>
   </si>
@@ -70,6 +70,123 @@
   </si>
   <si>
     <t>A-</t>
+  </si>
+  <si>
+    <t>doe@myschool.edu</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Doe</t>
+  </si>
+  <si>
+    <t>DATA201</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>smith@myschool.edu</t>
+  </si>
+  <si>
+    <t>Jane</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>DATA202</t>
+  </si>
+  <si>
+    <t>jones@myschool.edu</t>
+  </si>
+  <si>
+    <t>Emily</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>DATA203</t>
+  </si>
+  <si>
+    <t>brown@myschool.edu</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>DATA204</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>davis@myschool.edu</t>
+  </si>
+  <si>
+    <t>Sarah</t>
+  </si>
+  <si>
+    <t>Davis</t>
+  </si>
+  <si>
+    <t>miller@myschool.edu</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>C+</t>
+  </si>
+  <si>
+    <t>wilson@myschool.edu</t>
+  </si>
+  <si>
+    <t>Lucy</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>B-</t>
+  </si>
+  <si>
+    <t>moore@myschool.edu</t>
+  </si>
+  <si>
+    <t>Charles</t>
+  </si>
+  <si>
+    <t>Moore</t>
+  </si>
+  <si>
+    <t>taylor@myschool.edu</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>anderson@myschool.edu</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Anderson</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
@@ -114,9 +231,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -140,9 +263,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -180,7 +303,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -286,7 +409,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -428,7 +551,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -436,15 +559,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6C6B5B9-B226-488D-8B04-AC508BAF3B03}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" customWidth="1"/>
+    <col min="1" max="1" width="24" customWidth="1"/>
     <col min="2" max="2" width="15.54296875" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="9.90625" bestFit="1" customWidth="1"/>
@@ -452,7 +575,7 @@
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -472,7 +595,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -492,7 +615,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -511,6 +634,207 @@
       <c r="F3">
         <v>91</v>
       </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" s="2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="2">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="2">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F10" s="2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" s="2">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F13" s="2">
+        <v>75</v>
+      </c>
+      <c r="H13" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>